<commit_message>
Filter for account bills skipped in budged bills
It moved the logic from complex non-readable Excel formula into
the simple filterAccountBillsNotInBudgetBills() with filter() and some()

For this reason "status" column is not needed anymore.

To cover new logic, test data in accountBills.xlsx, budgetBills.xlsx,
and mocks.ts are adjusted,
</commit_message>
<xml_diff>
--- a/tests/resources/xlsx/accountBills copy.xlsx
+++ b/tests/resources/xlsx/accountBills copy.xlsx
@@ -5,17 +5,17 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\skipped-bills\tests\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\skipped-bills\tests\resources\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2299C21A-7B50-4B8C-A57E-74E93D85868A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA68413-14A1-4650-B99A-EEC1BCAB2C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transactions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -83,9 +83,6 @@
     <t>Transaction type</t>
   </si>
   <si>
-    <t>Prise</t>
-  </si>
-  <si>
     <t>Currency</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Amount</t>
   </si>
 </sst>
 </file>
@@ -189,47 +189,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{D210C99C-A905-4E41-A64D-F1CB2B864A2A}"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -248,10 +208,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -579,7 +535,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -601,19 +557,19 @@
         <v>3</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>15</v>
       </c>
       <c r="F1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -679,7 +635,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="5">
-        <v>44565</v>
+        <v>44566</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>10</v>
@@ -696,10 +652,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B4">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$F2&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>